<commit_message>
perbaiki hapus jurnal dan tambah
</commit_message>
<xml_diff>
--- a/data data/Data Bimbingan.xlsx
+++ b/data data/Data Bimbingan.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Cluster_Dosen\data data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\cluster_dosen\data data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D3C4150-266B-4DE3-BB9E-D8CE75415F0C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F636997E-6D18-4B9C-8A6C-2BB3649B7A69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="4" xr2:uid="{2A9C50C2-8366-4052-A1C5-A44B410141F3}"/>
   </bookViews>
@@ -7847,7 +7847,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -7951,8 +7951,26 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -7998,6 +8016,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor theme="0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor theme="0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -8088,7 +8136,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="126">
+  <cellXfs count="151">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -8340,16 +8388,10 @@
     <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -8361,10 +8403,71 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -8723,15 +8826,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" customHeight="1">
-      <c r="A1" s="124" t="s">
+      <c r="A1" s="131" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="125"/>
-      <c r="C1" s="125"/>
-      <c r="D1" s="125"/>
-      <c r="E1" s="125"/>
-      <c r="F1" s="125"/>
-      <c r="G1" s="125"/>
+      <c r="B1" s="132"/>
+      <c r="C1" s="132"/>
+      <c r="D1" s="132"/>
+      <c r="E1" s="132"/>
+      <c r="F1" s="132"/>
+      <c r="G1" s="132"/>
     </row>
     <row r="2" spans="1:21">
       <c r="B2" s="1"/>
@@ -11921,15 +12024,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="20.25">
-      <c r="A1" s="124" t="s">
+      <c r="A1" s="131" t="s">
         <v>318</v>
       </c>
-      <c r="B1" s="125"/>
-      <c r="C1" s="125"/>
-      <c r="D1" s="125"/>
-      <c r="E1" s="125"/>
-      <c r="F1" s="125"/>
-      <c r="G1" s="125"/>
+      <c r="B1" s="132"/>
+      <c r="C1" s="132"/>
+      <c r="D1" s="132"/>
+      <c r="E1" s="132"/>
+      <c r="F1" s="132"/>
+      <c r="G1" s="132"/>
     </row>
     <row r="2" spans="1:7">
       <c r="B2" s="1"/>
@@ -13160,15 +13263,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="23.25" customHeight="1">
-      <c r="A1" s="124" t="s">
+      <c r="A1" s="131" t="s">
         <v>482</v>
       </c>
-      <c r="B1" s="125"/>
-      <c r="C1" s="125"/>
-      <c r="D1" s="125"/>
-      <c r="E1" s="125"/>
-      <c r="F1" s="125"/>
-      <c r="G1" s="125"/>
+      <c r="B1" s="132"/>
+      <c r="C1" s="132"/>
+      <c r="D1" s="132"/>
+      <c r="E1" s="132"/>
+      <c r="F1" s="132"/>
+      <c r="G1" s="132"/>
     </row>
     <row r="2" spans="1:7">
       <c r="B2" s="1"/>
@@ -20355,15 +20458,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="23.25" customHeight="1">
-      <c r="A1" s="124" t="s">
+      <c r="A1" s="131" t="s">
         <v>482</v>
       </c>
-      <c r="B1" s="125"/>
-      <c r="C1" s="125"/>
-      <c r="D1" s="125"/>
-      <c r="E1" s="125"/>
-      <c r="F1" s="125"/>
-      <c r="G1" s="125"/>
+      <c r="B1" s="132"/>
+      <c r="C1" s="132"/>
+      <c r="D1" s="132"/>
+      <c r="E1" s="132"/>
+      <c r="F1" s="132"/>
+      <c r="G1" s="132"/>
     </row>
     <row r="2" spans="1:7">
       <c r="B2" s="1"/>
@@ -25697,8 +25800,8 @@
   <dimension ref="A1:X227"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I75" sqref="I75"/>
+      <pane ySplit="2" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M90" sqref="M90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.85546875" defaultRowHeight="15" customHeight="1"/>
@@ -25762,17 +25865,17 @@
       <c r="D3" s="32" t="s">
         <v>1723</v>
       </c>
-      <c r="E3" s="32" t="s">
+      <c r="E3" s="145" t="s">
         <v>1724</v>
       </c>
-      <c r="F3" s="33" t="s">
+      <c r="F3" s="146" t="s">
         <v>486</v>
       </c>
       <c r="G3" s="99"/>
       <c r="H3" s="34" t="s">
         <v>295</v>
       </c>
-      <c r="I3" s="34" t="s">
+      <c r="I3" s="115" t="s">
         <v>116</v>
       </c>
     </row>
@@ -25799,7 +25902,7 @@
       <c r="H4" s="34" t="s">
         <v>360</v>
       </c>
-      <c r="I4" s="117" t="s">
+      <c r="I4" s="115" t="s">
         <v>79</v>
       </c>
       <c r="J4" s="5"/>
@@ -25868,7 +25971,7 @@
       <c r="H6" s="102" t="s">
         <v>107</v>
       </c>
-      <c r="I6" s="117" t="s">
+      <c r="I6" s="115" t="s">
         <v>79</v>
       </c>
     </row>
@@ -25974,7 +26077,7 @@
       <c r="H10" s="34" t="s">
         <v>295</v>
       </c>
-      <c r="I10" s="117" t="s">
+      <c r="I10" s="115" t="s">
         <v>431</v>
       </c>
     </row>
@@ -26001,7 +26104,7 @@
       <c r="H11" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="I11" s="117" t="s">
+      <c r="I11" s="115" t="s">
         <v>45</v>
       </c>
     </row>
@@ -26025,7 +26128,7 @@
         <v>486</v>
       </c>
       <c r="G12" s="99"/>
-      <c r="H12" s="117" t="s">
+      <c r="H12" s="115" t="s">
         <v>328</v>
       </c>
       <c r="I12" s="34" t="s">
@@ -26055,7 +26158,7 @@
       <c r="H13" s="34" t="s">
         <v>295</v>
       </c>
-      <c r="I13" s="117" t="s">
+      <c r="I13" s="115" t="s">
         <v>193</v>
       </c>
     </row>
@@ -26072,14 +26175,14 @@
       <c r="D14" s="36" t="s">
         <v>1762</v>
       </c>
-      <c r="E14" s="37" t="s">
+      <c r="E14" s="114" t="s">
         <v>1763</v>
       </c>
-      <c r="F14" s="38" t="s">
+      <c r="F14" s="136" t="s">
         <v>486</v>
       </c>
       <c r="G14" s="99"/>
-      <c r="H14" s="34" t="s">
+      <c r="H14" s="115" t="s">
         <v>149</v>
       </c>
       <c r="I14" s="34" t="s">
@@ -26106,7 +26209,7 @@
         <v>486</v>
       </c>
       <c r="G15" s="99"/>
-      <c r="H15" s="114" t="s">
+      <c r="H15" s="113" t="s">
         <v>65</v>
       </c>
       <c r="I15" s="34" t="s">
@@ -26126,17 +26229,17 @@
       <c r="D16" s="37" t="s">
         <v>1771</v>
       </c>
-      <c r="E16" s="37" t="s">
+      <c r="E16" s="114" t="s">
         <v>1772</v>
       </c>
-      <c r="F16" s="38" t="s">
+      <c r="F16" s="136" t="s">
         <v>486</v>
       </c>
       <c r="G16" s="99"/>
-      <c r="H16" s="34" t="s">
+      <c r="H16" s="115" t="s">
         <v>488</v>
       </c>
-      <c r="I16" s="34" t="s">
+      <c r="I16" s="115" t="s">
         <v>561</v>
       </c>
     </row>
@@ -26160,10 +26263,10 @@
         <v>486</v>
       </c>
       <c r="G17" s="99"/>
-      <c r="H17" s="117" t="s">
+      <c r="H17" s="115" t="s">
         <v>59</v>
       </c>
-      <c r="I17" s="117" t="s">
+      <c r="I17" s="115" t="s">
         <v>79</v>
       </c>
     </row>
@@ -26187,7 +26290,7 @@
         <v>486</v>
       </c>
       <c r="G18" s="99"/>
-      <c r="H18" s="117" t="s">
+      <c r="H18" s="115" t="s">
         <v>128</v>
       </c>
       <c r="I18" s="34" t="s">
@@ -26241,7 +26344,7 @@
         <v>486</v>
       </c>
       <c r="G20" s="99"/>
-      <c r="H20" s="117" t="s">
+      <c r="H20" s="115" t="s">
         <v>65</v>
       </c>
       <c r="I20" s="34" t="s">
@@ -26268,7 +26371,7 @@
         <v>486</v>
       </c>
       <c r="G21" s="99"/>
-      <c r="H21" s="117" t="s">
+      <c r="H21" s="115" t="s">
         <v>128</v>
       </c>
       <c r="I21" s="34" t="s">
@@ -26298,7 +26401,7 @@
       <c r="H22" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="I22" s="117" t="s">
+      <c r="I22" s="115" t="s">
         <v>202</v>
       </c>
     </row>
@@ -26325,7 +26428,7 @@
       <c r="H23" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="I23" s="117" t="s">
+      <c r="I23" s="115" t="s">
         <v>328</v>
       </c>
     </row>
@@ -26342,14 +26445,14 @@
       <c r="D24" s="36" t="s">
         <v>1803</v>
       </c>
-      <c r="E24" s="36" t="s">
+      <c r="E24" s="138" t="s">
         <v>1804</v>
       </c>
-      <c r="F24" s="38" t="s">
+      <c r="F24" s="136" t="s">
         <v>486</v>
       </c>
       <c r="G24" s="99"/>
-      <c r="H24" s="117" t="s">
+      <c r="H24" s="115" t="s">
         <v>514</v>
       </c>
       <c r="I24" s="34" t="s">
@@ -26423,7 +26526,7 @@
       <c r="D27" s="68" t="s">
         <v>1814</v>
       </c>
-      <c r="E27" s="37" t="s">
+      <c r="E27" s="114" t="s">
         <v>1815</v>
       </c>
       <c r="F27" s="38" t="s">
@@ -26433,7 +26536,7 @@
       <c r="H27" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="I27" s="34" t="s">
+      <c r="I27" s="115" t="s">
         <v>469</v>
       </c>
     </row>
@@ -26457,7 +26560,7 @@
         <v>486</v>
       </c>
       <c r="G28" s="99"/>
-      <c r="H28" s="114" t="s">
+      <c r="H28" s="128" t="s">
         <v>141</v>
       </c>
       <c r="I28" s="34" t="s">
@@ -26511,10 +26614,10 @@
         <v>486</v>
       </c>
       <c r="G30" s="99"/>
-      <c r="H30" s="117" t="s">
+      <c r="H30" s="115" t="s">
         <v>65</v>
       </c>
-      <c r="I30" s="117" t="s">
+      <c r="I30" s="126" t="s">
         <v>22</v>
       </c>
     </row>
@@ -26595,7 +26698,7 @@
       <c r="H33" s="102" t="s">
         <v>360</v>
       </c>
-      <c r="I33" s="114" t="s">
+      <c r="I33" s="113" t="s">
         <v>328</v>
       </c>
     </row>
@@ -26619,7 +26722,7 @@
         <v>486</v>
       </c>
       <c r="G34" s="99"/>
-      <c r="H34" s="117" t="s">
+      <c r="H34" s="115" t="s">
         <v>60</v>
       </c>
       <c r="I34" s="34" t="s">
@@ -26646,10 +26749,10 @@
         <v>486</v>
       </c>
       <c r="G35" s="99"/>
-      <c r="H35" s="117" t="s">
+      <c r="H35" s="122" t="s">
         <v>64</v>
       </c>
-      <c r="I35" s="117" t="s">
+      <c r="I35" s="115" t="s">
         <v>60</v>
       </c>
     </row>
@@ -26676,7 +26779,7 @@
       <c r="H36" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="I36" s="117" t="s">
+      <c r="I36" s="126" t="s">
         <v>22</v>
       </c>
     </row>
@@ -26747,14 +26850,14 @@
       <c r="D39" s="37" t="s">
         <v>1860</v>
       </c>
-      <c r="E39" s="37" t="s">
+      <c r="E39" s="114" t="s">
         <v>1861</v>
       </c>
-      <c r="F39" s="38" t="s">
+      <c r="F39" s="139" t="s">
         <v>486</v>
       </c>
       <c r="G39" s="99"/>
-      <c r="H39" s="34" t="s">
+      <c r="H39" s="115" t="s">
         <v>488</v>
       </c>
       <c r="I39" s="34" t="s">
@@ -26781,10 +26884,10 @@
         <v>486</v>
       </c>
       <c r="G40" s="99"/>
-      <c r="H40" s="117" t="s">
+      <c r="H40" s="122" t="s">
         <v>120</v>
       </c>
-      <c r="I40" s="117" t="s">
+      <c r="I40" s="115" t="s">
         <v>287</v>
       </c>
     </row>
@@ -26811,7 +26914,7 @@
       <c r="H41" s="34" t="s">
         <v>96</v>
       </c>
-      <c r="I41" s="117" t="s">
+      <c r="I41" s="126" t="s">
         <v>36</v>
       </c>
     </row>
@@ -26835,10 +26938,10 @@
         <v>486</v>
       </c>
       <c r="G42" s="99"/>
-      <c r="H42" s="117" t="s">
+      <c r="H42" s="115" t="s">
         <v>12</v>
       </c>
-      <c r="I42" s="117" t="s">
+      <c r="I42" s="115" t="s">
         <v>253</v>
       </c>
     </row>
@@ -26862,7 +26965,7 @@
         <v>486</v>
       </c>
       <c r="G43" s="99"/>
-      <c r="H43" s="117" t="s">
+      <c r="H43" s="115" t="s">
         <v>73</v>
       </c>
       <c r="I43" s="34" t="s">
@@ -26916,7 +27019,7 @@
         <v>486</v>
       </c>
       <c r="G45" s="99"/>
-      <c r="H45" s="117" t="s">
+      <c r="H45" s="122" t="s">
         <v>316</v>
       </c>
       <c r="I45" s="34" t="s">
@@ -26963,17 +27066,17 @@
       <c r="D47" s="36" t="s">
         <v>1892</v>
       </c>
-      <c r="E47" s="37" t="s">
+      <c r="E47" s="114" t="s">
         <v>1893</v>
       </c>
-      <c r="F47" s="38" t="s">
+      <c r="F47" s="139" t="s">
         <v>486</v>
       </c>
       <c r="G47" s="99"/>
-      <c r="H47" s="117" t="s">
+      <c r="H47" s="115" t="s">
         <v>514</v>
       </c>
-      <c r="I47" s="117" t="s">
+      <c r="I47" s="115" t="s">
         <v>1711</v>
       </c>
     </row>
@@ -27027,7 +27130,7 @@
       <c r="H49" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="I49" s="117" t="s">
+      <c r="I49" s="115" t="s">
         <v>1711</v>
       </c>
     </row>
@@ -27071,14 +27174,14 @@
       <c r="D51" s="37" t="s">
         <v>1908</v>
       </c>
-      <c r="E51" s="37" t="s">
+      <c r="E51" s="114" t="s">
         <v>1909</v>
       </c>
-      <c r="F51" s="38" t="s">
+      <c r="F51" s="139" t="s">
         <v>486</v>
       </c>
       <c r="G51" s="99"/>
-      <c r="H51" s="34" t="s">
+      <c r="H51" s="115" t="s">
         <v>488</v>
       </c>
       <c r="I51" s="34" t="s">
@@ -27132,7 +27235,7 @@
         <v>486</v>
       </c>
       <c r="G53" s="71"/>
-      <c r="H53" s="117" t="s">
+      <c r="H53" s="115" t="s">
         <v>65</v>
       </c>
       <c r="I53" s="34" t="s">
@@ -27177,7 +27280,7 @@
       <c r="H54" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="I54" s="117" t="s">
+      <c r="I54" s="126" t="s">
         <v>36</v>
       </c>
     </row>
@@ -27231,7 +27334,7 @@
       <c r="H56" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="I56" s="117" t="s">
+      <c r="I56" s="126" t="s">
         <v>22</v>
       </c>
     </row>
@@ -27255,7 +27358,7 @@
         <v>486</v>
       </c>
       <c r="G57" s="99"/>
-      <c r="H57" s="117" t="s">
+      <c r="H57" s="122" t="s">
         <v>120</v>
       </c>
       <c r="I57" s="34" t="s">
@@ -27282,10 +27385,10 @@
         <v>486</v>
       </c>
       <c r="G58" s="99"/>
-      <c r="H58" s="117" t="s">
+      <c r="H58" s="115" t="s">
         <v>45</v>
       </c>
-      <c r="I58" s="117" t="s">
+      <c r="I58" s="115" t="s">
         <v>12</v>
       </c>
     </row>
@@ -27309,7 +27412,7 @@
         <v>486</v>
       </c>
       <c r="G59" s="99"/>
-      <c r="H59" s="117" t="s">
+      <c r="H59" s="122" t="s">
         <v>120</v>
       </c>
       <c r="I59" s="34" t="s">
@@ -27329,14 +27432,14 @@
       <c r="D60" s="37" t="s">
         <v>1944</v>
       </c>
-      <c r="E60" s="37" t="s">
+      <c r="E60" s="114" t="s">
         <v>1945</v>
       </c>
-      <c r="F60" s="38" t="s">
+      <c r="F60" s="136" t="s">
         <v>486</v>
       </c>
       <c r="G60" s="99"/>
-      <c r="H60" s="34" t="s">
+      <c r="H60" s="115" t="s">
         <v>106</v>
       </c>
       <c r="I60" s="34" t="s">
@@ -27366,7 +27469,7 @@
       <c r="H61" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="I61" s="117" t="s">
+      <c r="I61" s="122" t="s">
         <v>74</v>
       </c>
     </row>
@@ -27390,10 +27493,10 @@
         <v>486</v>
       </c>
       <c r="G62" s="99"/>
-      <c r="H62" s="34" t="s">
+      <c r="H62" s="115" t="s">
         <v>27</v>
       </c>
-      <c r="I62" s="120" t="s">
+      <c r="I62" s="118" t="s">
         <v>1952</v>
       </c>
     </row>
@@ -27417,10 +27520,10 @@
         <v>486</v>
       </c>
       <c r="G63" s="99"/>
-      <c r="H63" s="117" t="s">
+      <c r="H63" s="115" t="s">
         <v>59</v>
       </c>
-      <c r="I63" s="117" t="s">
+      <c r="I63" s="115" t="s">
         <v>202</v>
       </c>
     </row>
@@ -27498,7 +27601,7 @@
         <v>486</v>
       </c>
       <c r="G66" s="99"/>
-      <c r="H66" s="114" t="s">
+      <c r="H66" s="128" t="s">
         <v>141</v>
       </c>
       <c r="I66" s="34" t="s">
@@ -27525,7 +27628,7 @@
         <v>486</v>
       </c>
       <c r="G67" s="99"/>
-      <c r="H67" s="117" t="s">
+      <c r="H67" s="122" t="s">
         <v>316</v>
       </c>
       <c r="I67" s="34" t="s">
@@ -27552,7 +27655,7 @@
         <v>486</v>
       </c>
       <c r="G68" s="99"/>
-      <c r="H68" s="117" t="s">
+      <c r="H68" s="115" t="s">
         <v>59</v>
       </c>
       <c r="I68" s="34" t="s">
@@ -27572,14 +27675,14 @@
       <c r="D69" s="37" t="s">
         <v>1979</v>
       </c>
-      <c r="E69" s="37" t="s">
+      <c r="E69" s="114" t="s">
         <v>1980</v>
       </c>
       <c r="F69" s="38" t="s">
         <v>486</v>
       </c>
       <c r="G69" s="99"/>
-      <c r="H69" s="34" t="s">
+      <c r="H69" s="115" t="s">
         <v>27</v>
       </c>
       <c r="I69" s="34" t="s">
@@ -27609,7 +27712,7 @@
       <c r="H70" s="34" t="s">
         <v>270</v>
       </c>
-      <c r="I70" s="117" t="s">
+      <c r="I70" s="115" t="s">
         <v>287</v>
       </c>
     </row>
@@ -27626,7 +27729,7 @@
       <c r="D71" s="37" t="s">
         <v>1986</v>
       </c>
-      <c r="E71" s="37" t="s">
+      <c r="E71" s="114" t="s">
         <v>1987</v>
       </c>
       <c r="F71" s="103" t="s">
@@ -27636,7 +27739,7 @@
       <c r="H71" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="I71" s="34" t="s">
+      <c r="I71" s="115" t="s">
         <v>41</v>
       </c>
     </row>
@@ -27660,10 +27763,10 @@
         <v>486</v>
       </c>
       <c r="G72" s="99"/>
-      <c r="H72" s="114" t="s">
+      <c r="H72" s="113" t="s">
         <v>328</v>
       </c>
-      <c r="I72" s="117" t="s">
+      <c r="I72" s="115" t="s">
         <v>202</v>
       </c>
     </row>
@@ -27687,10 +27790,10 @@
         <v>486</v>
       </c>
       <c r="G73" s="99"/>
-      <c r="H73" s="117" t="s">
+      <c r="H73" s="115" t="s">
         <v>128</v>
       </c>
-      <c r="I73" s="117" t="s">
+      <c r="I73" s="122" t="s">
         <v>74</v>
       </c>
     </row>
@@ -27717,7 +27820,7 @@
       <c r="H74" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="I74" s="117" t="s">
+      <c r="I74" s="115" t="s">
         <v>287</v>
       </c>
     </row>
@@ -27744,7 +27847,7 @@
       <c r="H75" s="34" t="s">
         <v>270</v>
       </c>
-      <c r="I75" s="117" t="s">
+      <c r="I75" s="115" t="s">
         <v>60</v>
       </c>
     </row>
@@ -27761,17 +27864,17 @@
       <c r="D76" s="37" t="s">
         <v>2005</v>
       </c>
-      <c r="E76" s="37" t="s">
+      <c r="E76" s="114" t="s">
         <v>2006</v>
       </c>
-      <c r="F76" s="38" t="s">
+      <c r="F76" s="139" t="s">
         <v>486</v>
       </c>
       <c r="G76" s="99"/>
       <c r="H76" s="34" t="s">
         <v>360</v>
       </c>
-      <c r="I76" s="34" t="s">
+      <c r="I76" s="147" t="s">
         <v>116</v>
       </c>
     </row>
@@ -27795,7 +27898,7 @@
         <v>486</v>
       </c>
       <c r="G77" s="99"/>
-      <c r="H77" s="114" t="s">
+      <c r="H77" s="128" t="s">
         <v>36</v>
       </c>
       <c r="I77" s="102" t="s">
@@ -27876,7 +27979,7 @@
         <v>486</v>
       </c>
       <c r="G80" s="99"/>
-      <c r="H80" s="117" t="s">
+      <c r="H80" s="122" t="s">
         <v>316</v>
       </c>
       <c r="I80" s="34" t="s">
@@ -27896,17 +27999,17 @@
       <c r="D81" s="37" t="s">
         <v>2023</v>
       </c>
-      <c r="E81" s="36" t="s">
+      <c r="E81" s="138" t="s">
         <v>2024</v>
       </c>
-      <c r="F81" s="38" t="s">
+      <c r="F81" s="139" t="s">
         <v>486</v>
       </c>
       <c r="G81" s="99"/>
       <c r="H81" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="I81" s="34" t="s">
+      <c r="I81" s="115" t="s">
         <v>129</v>
       </c>
     </row>
@@ -27930,7 +28033,7 @@
         <v>486</v>
       </c>
       <c r="G82" s="99"/>
-      <c r="H82" s="117" t="s">
+      <c r="H82" s="126" t="s">
         <v>36</v>
       </c>
       <c r="I82" s="34" t="s">
@@ -27950,14 +28053,14 @@
       <c r="D83" s="36" t="s">
         <v>2031</v>
       </c>
-      <c r="E83" s="37" t="s">
+      <c r="E83" s="114" t="s">
         <v>2032</v>
       </c>
       <c r="F83" s="38" t="s">
         <v>486</v>
       </c>
       <c r="G83" s="99"/>
-      <c r="H83" s="34" t="s">
+      <c r="H83" s="115" t="s">
         <v>149</v>
       </c>
       <c r="I83" s="34" t="s">
@@ -28014,7 +28117,7 @@
       <c r="H85" s="34" t="s">
         <v>357</v>
       </c>
-      <c r="I85" s="117" t="s">
+      <c r="I85" s="115" t="s">
         <v>431</v>
       </c>
     </row>
@@ -28038,7 +28141,7 @@
         <v>486</v>
       </c>
       <c r="G86" s="99"/>
-      <c r="H86" s="114" t="s">
+      <c r="H86" s="128" t="s">
         <v>141</v>
       </c>
       <c r="I86" s="34" t="s">
@@ -28065,7 +28168,7 @@
         <v>486</v>
       </c>
       <c r="G87" s="99"/>
-      <c r="H87" s="117" t="s">
+      <c r="H87" s="115" t="s">
         <v>64</v>
       </c>
       <c r="I87" s="34" t="s">
@@ -28092,7 +28195,7 @@
         <v>486</v>
       </c>
       <c r="G88" s="99"/>
-      <c r="H88" s="117" t="s">
+      <c r="H88" s="115" t="s">
         <v>45</v>
       </c>
       <c r="I88" s="34" t="s">
@@ -28139,14 +28242,14 @@
       <c r="D90" s="37" t="s">
         <v>2058</v>
       </c>
-      <c r="E90" s="37" t="s">
+      <c r="E90" s="114" t="s">
         <v>2059</v>
       </c>
       <c r="F90" s="38" t="s">
         <v>486</v>
       </c>
       <c r="G90" s="99"/>
-      <c r="H90" s="34" t="s">
+      <c r="H90" s="115" t="s">
         <v>149</v>
       </c>
       <c r="I90" s="34" t="s">
@@ -28166,17 +28269,17 @@
       <c r="D91" s="37" t="s">
         <v>2062</v>
       </c>
-      <c r="E91" s="115" t="s">
+      <c r="E91" s="114" t="s">
         <v>2063</v>
       </c>
       <c r="F91" s="38" t="s">
         <v>486</v>
       </c>
       <c r="G91" s="99"/>
-      <c r="H91" s="114" t="s">
+      <c r="H91" s="124" t="s">
         <v>291</v>
       </c>
-      <c r="I91" s="34" t="s">
+      <c r="I91" s="115" t="s">
         <v>561</v>
       </c>
     </row>
@@ -28203,7 +28306,7 @@
       <c r="H92" s="34" t="s">
         <v>124</v>
       </c>
-      <c r="I92" s="117" t="s">
+      <c r="I92" s="115" t="s">
         <v>92</v>
       </c>
     </row>
@@ -28225,7 +28328,7 @@
         <v>486</v>
       </c>
       <c r="G93" s="40"/>
-      <c r="H93" s="120" t="s">
+      <c r="H93" s="118" t="s">
         <v>73</v>
       </c>
       <c r="I93" s="40" t="s">
@@ -28294,7 +28397,7 @@
         <v>486</v>
       </c>
       <c r="G95" s="99"/>
-      <c r="H95" s="114" t="s">
+      <c r="H95" s="113" t="s">
         <v>12</v>
       </c>
       <c r="I95" s="102" t="s">
@@ -28314,17 +28417,17 @@
       <c r="D96" s="37" t="s">
         <v>2080</v>
       </c>
-      <c r="E96" s="115" t="s">
+      <c r="E96" s="114" t="s">
         <v>2081</v>
       </c>
       <c r="F96" s="38" t="s">
         <v>486</v>
       </c>
       <c r="G96" s="99"/>
-      <c r="H96" s="114" t="s">
+      <c r="H96" s="124" t="s">
         <v>291</v>
       </c>
-      <c r="I96" s="40" t="s">
+      <c r="I96" s="118" t="s">
         <v>149</v>
       </c>
     </row>
@@ -28341,14 +28444,14 @@
       <c r="D97" s="37" t="s">
         <v>2084</v>
       </c>
-      <c r="E97" s="115" t="s">
+      <c r="E97" s="114" t="s">
         <v>2085</v>
       </c>
       <c r="F97" s="38" t="s">
         <v>486</v>
       </c>
       <c r="G97" s="99"/>
-      <c r="H97" s="116" t="s">
+      <c r="H97" s="125" t="s">
         <v>291</v>
       </c>
       <c r="I97" s="34" t="s">
@@ -28375,7 +28478,7 @@
         <v>486</v>
       </c>
       <c r="G98" s="99"/>
-      <c r="H98" s="117" t="s">
+      <c r="H98" s="115" t="s">
         <v>64</v>
       </c>
       <c r="I98" s="34" t="s">
@@ -28432,7 +28535,7 @@
       <c r="H100" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="I100" s="117" t="s">
+      <c r="I100" s="115" t="s">
         <v>193</v>
       </c>
     </row>
@@ -28510,7 +28613,7 @@
         <v>486</v>
       </c>
       <c r="G103" s="99"/>
-      <c r="H103" s="117" t="s">
+      <c r="H103" s="115" t="s">
         <v>65</v>
       </c>
       <c r="I103" s="34" t="s">
@@ -28530,17 +28633,17 @@
       <c r="D104" s="37" t="s">
         <v>2111</v>
       </c>
-      <c r="E104" s="37" t="s">
+      <c r="E104" s="114" t="s">
         <v>2112</v>
       </c>
-      <c r="F104" s="38" t="s">
+      <c r="F104" s="136" t="s">
         <v>486</v>
       </c>
       <c r="G104" s="99"/>
-      <c r="H104" s="117" t="s">
+      <c r="H104" s="115" t="s">
         <v>59</v>
       </c>
-      <c r="I104" s="34" t="s">
+      <c r="I104" s="115" t="s">
         <v>488</v>
       </c>
     </row>
@@ -28564,7 +28667,7 @@
         <v>486</v>
       </c>
       <c r="G105" s="99"/>
-      <c r="H105" s="114" t="s">
+      <c r="H105" s="128" t="s">
         <v>141</v>
       </c>
       <c r="I105" s="34" t="s">
@@ -28584,17 +28687,17 @@
       <c r="D106" s="37" t="s">
         <v>2119</v>
       </c>
-      <c r="E106" s="37" t="s">
+      <c r="E106" s="114" t="s">
         <v>2120</v>
       </c>
       <c r="F106" s="38" t="s">
         <v>486</v>
       </c>
       <c r="G106" s="99"/>
-      <c r="H106" s="34" t="s">
+      <c r="H106" s="115" t="s">
         <v>27</v>
       </c>
-      <c r="I106" s="117" t="s">
+      <c r="I106" s="115" t="s">
         <v>79</v>
       </c>
     </row>
@@ -28611,17 +28714,17 @@
       <c r="D107" s="37" t="s">
         <v>2123</v>
       </c>
-      <c r="E107" s="37" t="s">
+      <c r="E107" s="114" t="s">
         <v>2124</v>
       </c>
-      <c r="F107" s="38" t="s">
+      <c r="F107" s="139" t="s">
         <v>486</v>
       </c>
       <c r="G107" s="99"/>
       <c r="H107" s="102" t="s">
         <v>31</v>
       </c>
-      <c r="I107" s="34" t="s">
+      <c r="I107" s="115" t="s">
         <v>111</v>
       </c>
     </row>
@@ -28645,10 +28748,10 @@
         <v>486</v>
       </c>
       <c r="G108" s="99"/>
-      <c r="H108" s="117" t="s">
+      <c r="H108" s="115" t="s">
         <v>59</v>
       </c>
-      <c r="I108" s="117" t="s">
+      <c r="I108" s="115" t="s">
         <v>12</v>
       </c>
     </row>
@@ -28675,7 +28778,7 @@
       <c r="H109" s="34" t="s">
         <v>107</v>
       </c>
-      <c r="I109" s="117" t="s">
+      <c r="I109" s="115" t="s">
         <v>92</v>
       </c>
     </row>
@@ -28699,7 +28802,7 @@
         <v>486</v>
       </c>
       <c r="G110" s="99"/>
-      <c r="H110" s="117" t="s">
+      <c r="H110" s="115" t="s">
         <v>45</v>
       </c>
       <c r="I110" s="34" t="s">
@@ -28726,7 +28829,7 @@
         <v>486</v>
       </c>
       <c r="G111" s="99"/>
-      <c r="H111" s="34" t="s">
+      <c r="H111" s="122" t="s">
         <v>102</v>
       </c>
       <c r="I111" s="34" t="s">
@@ -28771,7 +28874,7 @@
       <c r="H112" s="34" t="s">
         <v>124</v>
       </c>
-      <c r="I112" s="117" t="s">
+      <c r="I112" s="115" t="s">
         <v>133</v>
       </c>
     </row>
@@ -28798,7 +28901,7 @@
       <c r="H113" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="I113" s="117" t="s">
+      <c r="I113" s="115" t="s">
         <v>253</v>
       </c>
     </row>
@@ -28825,7 +28928,7 @@
       <c r="H114" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="I114" s="117" t="s">
+      <c r="I114" s="115" t="s">
         <v>193</v>
       </c>
     </row>
@@ -28849,7 +28952,7 @@
         <v>486</v>
       </c>
       <c r="G115" s="99"/>
-      <c r="H115" s="117" t="s">
+      <c r="H115" s="126" t="s">
         <v>22</v>
       </c>
       <c r="I115" s="34" t="s">
@@ -28869,17 +28972,17 @@
       <c r="D116" s="36" t="s">
         <v>2159</v>
       </c>
-      <c r="E116" s="115" t="s">
+      <c r="E116" s="114" t="s">
         <v>2160</v>
       </c>
       <c r="F116" s="38" t="s">
         <v>486</v>
       </c>
       <c r="G116" s="99"/>
-      <c r="H116" s="117" t="s">
+      <c r="H116" s="122" t="s">
         <v>291</v>
       </c>
-      <c r="I116" s="117" t="s">
+      <c r="I116" s="115" t="s">
         <v>92</v>
       </c>
     </row>
@@ -28903,7 +29006,7 @@
         <v>486</v>
       </c>
       <c r="G117" s="99"/>
-      <c r="H117" s="117" t="s">
+      <c r="H117" s="115" t="s">
         <v>59</v>
       </c>
       <c r="I117" s="34" t="s">
@@ -28957,7 +29060,7 @@
         <v>486</v>
       </c>
       <c r="G119" s="99"/>
-      <c r="H119" s="117" t="s">
+      <c r="H119" s="115" t="s">
         <v>59</v>
       </c>
       <c r="I119" s="34" t="s">
@@ -28984,10 +29087,10 @@
         <v>486</v>
       </c>
       <c r="G120" s="99"/>
-      <c r="H120" s="117" t="s">
+      <c r="H120" s="122" t="s">
         <v>316</v>
       </c>
-      <c r="I120" s="117" t="s">
+      <c r="I120" s="122" t="s">
         <v>74</v>
       </c>
     </row>
@@ -29014,7 +29117,7 @@
       <c r="H121" s="34" t="s">
         <v>124</v>
       </c>
-      <c r="I121" s="117" t="s">
+      <c r="I121" s="115" t="s">
         <v>133</v>
       </c>
     </row>
@@ -29065,7 +29168,7 @@
         <v>486</v>
       </c>
       <c r="G123" s="99"/>
-      <c r="H123" s="34" t="s">
+      <c r="H123" s="122" t="s">
         <v>102</v>
       </c>
       <c r="I123" s="102" t="s">
@@ -29085,14 +29188,14 @@
       <c r="D124" s="37" t="s">
         <v>2190</v>
       </c>
-      <c r="E124" s="37" t="s">
+      <c r="E124" s="114" t="s">
         <v>2191</v>
       </c>
-      <c r="F124" s="38" t="s">
+      <c r="F124" s="136" t="s">
         <v>486</v>
       </c>
       <c r="G124" s="99"/>
-      <c r="H124" s="34" t="s">
+      <c r="H124" s="115" t="s">
         <v>27</v>
       </c>
       <c r="I124" s="34" t="s">
@@ -29112,17 +29215,17 @@
       <c r="D125" s="36" t="s">
         <v>2194</v>
       </c>
-      <c r="E125" s="37" t="s">
+      <c r="E125" s="114" t="s">
         <v>2195</v>
       </c>
-      <c r="F125" s="38" t="s">
+      <c r="F125" s="136" t="s">
         <v>486</v>
       </c>
       <c r="G125" s="99"/>
-      <c r="H125" s="34" t="s">
+      <c r="H125" s="115" t="s">
         <v>149</v>
       </c>
-      <c r="I125" s="34" t="s">
+      <c r="I125" s="115" t="s">
         <v>129</v>
       </c>
     </row>
@@ -29139,17 +29242,17 @@
       <c r="D126" s="36" t="s">
         <v>2198</v>
       </c>
-      <c r="E126" s="37" t="s">
+      <c r="E126" s="114" t="s">
         <v>2199</v>
       </c>
-      <c r="F126" s="38" t="s">
+      <c r="F126" s="136" t="s">
         <v>486</v>
       </c>
       <c r="G126" s="99"/>
       <c r="H126" s="34" t="s">
         <v>96</v>
       </c>
-      <c r="I126" s="34" t="s">
+      <c r="I126" s="115" t="s">
         <v>469</v>
       </c>
     </row>
@@ -29166,7 +29269,7 @@
       <c r="D127" s="68" t="s">
         <v>2201</v>
       </c>
-      <c r="E127" s="37" t="s">
+      <c r="E127" s="114" t="s">
         <v>2202</v>
       </c>
       <c r="F127" s="38" t="s">
@@ -29176,7 +29279,7 @@
       <c r="H127" s="34" t="s">
         <v>270</v>
       </c>
-      <c r="I127" s="34" t="s">
+      <c r="I127" s="115" t="s">
         <v>561</v>
       </c>
     </row>
@@ -29283,7 +29386,7 @@
       <c r="G131" s="23" t="s">
         <v>2218</v>
       </c>
-      <c r="H131" s="121" t="s">
+      <c r="H131" s="129" t="s">
         <v>141</v>
       </c>
       <c r="I131" s="21" t="s">
@@ -29318,7 +29421,7 @@
       <c r="D132" s="50" t="s">
         <v>2221</v>
       </c>
-      <c r="E132" s="52" t="s">
+      <c r="E132" s="134" t="s">
         <v>2222</v>
       </c>
       <c r="F132" s="41" t="s">
@@ -29327,10 +29430,10 @@
       <c r="G132" s="21" t="s">
         <v>2223</v>
       </c>
-      <c r="H132" s="21" t="s">
+      <c r="H132" s="116" t="s">
         <v>149</v>
       </c>
-      <c r="I132" s="118" t="s">
+      <c r="I132" s="116" t="s">
         <v>60</v>
       </c>
     </row>
@@ -29347,16 +29450,16 @@
       <c r="D133" s="50" t="s">
         <v>2226</v>
       </c>
-      <c r="E133" s="52" t="s">
+      <c r="E133" s="134" t="s">
         <v>2227</v>
       </c>
-      <c r="F133" s="41" t="s">
+      <c r="F133" s="142" t="s">
         <v>10</v>
       </c>
       <c r="G133" s="21" t="s">
         <v>2218</v>
       </c>
-      <c r="H133" s="21" t="s">
+      <c r="H133" s="116" t="s">
         <v>149</v>
       </c>
       <c r="I133" s="21" t="s">
@@ -29388,7 +29491,7 @@
       <c r="H134" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="I134" s="118" t="s">
+      <c r="I134" s="116" t="s">
         <v>92</v>
       </c>
     </row>
@@ -29434,10 +29537,10 @@
       <c r="D136" s="107" t="s">
         <v>2238</v>
       </c>
-      <c r="E136" s="52" t="s">
+      <c r="E136" s="134" t="s">
         <v>2239</v>
       </c>
-      <c r="F136" s="41" t="s">
+      <c r="F136" s="143" t="s">
         <v>10</v>
       </c>
       <c r="G136" s="21" t="s">
@@ -29446,7 +29549,7 @@
       <c r="H136" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="I136" s="21" t="s">
+      <c r="I136" s="116" t="s">
         <v>116</v>
       </c>
     </row>
@@ -29472,7 +29575,7 @@
       <c r="G137" s="21" t="s">
         <v>2218</v>
       </c>
-      <c r="H137" s="118" t="s">
+      <c r="H137" s="127" t="s">
         <v>22</v>
       </c>
       <c r="I137" s="21" t="s">
@@ -29501,7 +29604,7 @@
       <c r="G138" s="21" t="s">
         <v>2248</v>
       </c>
-      <c r="H138" s="118" t="s">
+      <c r="H138" s="116" t="s">
         <v>328</v>
       </c>
       <c r="I138" s="21" t="s">
@@ -29530,7 +29633,7 @@
       <c r="G139" s="21" t="s">
         <v>2248</v>
       </c>
-      <c r="H139" s="118" t="s">
+      <c r="H139" s="116" t="s">
         <v>64</v>
       </c>
       <c r="I139" s="21" t="s">
@@ -29559,7 +29662,7 @@
       <c r="G140" s="21" t="s">
         <v>2223</v>
       </c>
-      <c r="H140" s="118" t="s">
+      <c r="H140" s="116" t="s">
         <v>45</v>
       </c>
       <c r="I140" s="21" t="s">
@@ -29591,7 +29694,7 @@
       <c r="H141" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="I141" s="123" t="s">
+      <c r="I141" s="121" t="s">
         <v>287</v>
       </c>
     </row>
@@ -29608,7 +29711,7 @@
       <c r="D142" s="50" t="s">
         <v>2264</v>
       </c>
-      <c r="E142" s="119" t="s">
+      <c r="E142" s="117" t="s">
         <v>2265</v>
       </c>
       <c r="F142" s="20" t="s">
@@ -29617,10 +29720,10 @@
       <c r="G142" s="21" t="s">
         <v>2261</v>
       </c>
-      <c r="H142" s="118" t="s">
+      <c r="H142" s="123" t="s">
         <v>291</v>
       </c>
-      <c r="I142" s="118" t="s">
+      <c r="I142" s="116" t="s">
         <v>1711</v>
       </c>
     </row>
@@ -29637,16 +29740,16 @@
       <c r="D143" s="50" t="s">
         <v>2268</v>
       </c>
-      <c r="E143" s="19" t="s">
+      <c r="E143" s="149" t="s">
         <v>2269</v>
       </c>
-      <c r="F143" s="20" t="s">
+      <c r="F143" s="144" t="s">
         <v>10</v>
       </c>
       <c r="G143" s="21" t="s">
         <v>2270</v>
       </c>
-      <c r="H143" s="21" t="s">
+      <c r="H143" s="116" t="s">
         <v>27</v>
       </c>
       <c r="I143" s="21" t="s">
@@ -29675,10 +29778,10 @@
       <c r="G144" s="21" t="s">
         <v>2274</v>
       </c>
-      <c r="H144" s="118" t="s">
+      <c r="H144" s="116" t="s">
         <v>59</v>
       </c>
-      <c r="I144" s="21" t="s">
+      <c r="I144" s="116" t="s">
         <v>129</v>
       </c>
     </row>
@@ -29704,7 +29807,7 @@
       <c r="G145" s="21" t="s">
         <v>2270</v>
       </c>
-      <c r="H145" s="118" t="s">
+      <c r="H145" s="116" t="s">
         <v>12</v>
       </c>
       <c r="I145" s="21" t="s">
@@ -29753,7 +29856,7 @@
       <c r="D147" s="50" t="s">
         <v>2285</v>
       </c>
-      <c r="E147" s="119" t="s">
+      <c r="E147" s="117" t="s">
         <v>2286</v>
       </c>
       <c r="F147" s="20" t="s">
@@ -29762,7 +29865,7 @@
       <c r="G147" s="40" t="s">
         <v>2261</v>
       </c>
-      <c r="H147" s="118" t="s">
+      <c r="H147" s="123" t="s">
         <v>291</v>
       </c>
       <c r="I147" s="21" t="s">
@@ -29811,7 +29914,7 @@
       <c r="D149" s="50" t="s">
         <v>2294</v>
       </c>
-      <c r="E149" s="119" t="s">
+      <c r="E149" s="117" t="s">
         <v>2295</v>
       </c>
       <c r="F149" s="20" t="s">
@@ -29823,7 +29926,7 @@
       <c r="H149" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="I149" s="118" t="s">
+      <c r="I149" s="123" t="s">
         <v>291</v>
       </c>
     </row>
@@ -29849,7 +29952,7 @@
       <c r="G150" s="21" t="s">
         <v>2218</v>
       </c>
-      <c r="H150" s="118" t="s">
+      <c r="H150" s="116" t="s">
         <v>328</v>
       </c>
       <c r="I150" s="21" t="s">
@@ -29881,7 +29984,7 @@
       <c r="H151" s="21" t="s">
         <v>1683</v>
       </c>
-      <c r="I151" s="118" t="s">
+      <c r="I151" s="116" t="s">
         <v>133</v>
       </c>
     </row>
@@ -29898,19 +30001,19 @@
       <c r="D152" s="52" t="s">
         <v>2307</v>
       </c>
-      <c r="E152" s="18" t="s">
+      <c r="E152" s="117" t="s">
         <v>2308</v>
       </c>
-      <c r="F152" s="20" t="s">
+      <c r="F152" s="133" t="s">
         <v>10</v>
       </c>
       <c r="G152" s="21" t="s">
         <v>2248</v>
       </c>
-      <c r="H152" s="21" t="s">
+      <c r="H152" s="116" t="s">
         <v>106</v>
       </c>
-      <c r="I152" s="21" t="s">
+      <c r="I152" s="116" t="s">
         <v>41</v>
       </c>
     </row>
@@ -29927,7 +30030,7 @@
       <c r="D153" s="50" t="s">
         <v>2311</v>
       </c>
-      <c r="E153" s="18" t="s">
+      <c r="E153" s="117" t="s">
         <v>2312</v>
       </c>
       <c r="F153" s="20" t="s">
@@ -29936,10 +30039,10 @@
       <c r="G153" s="40" t="s">
         <v>2313</v>
       </c>
-      <c r="H153" s="120" t="s">
+      <c r="H153" s="118" t="s">
         <v>73</v>
       </c>
-      <c r="I153" s="21" t="s">
+      <c r="I153" s="116" t="s">
         <v>129</v>
       </c>
     </row>
@@ -29965,7 +30068,7 @@
       <c r="G154" s="21" t="s">
         <v>2218</v>
       </c>
-      <c r="H154" s="120" t="s">
+      <c r="H154" s="118" t="s">
         <v>328</v>
       </c>
       <c r="I154" s="21" t="s">
@@ -30000,7 +30103,7 @@
       <c r="D155" s="50" t="s">
         <v>2320</v>
       </c>
-      <c r="E155" s="18" t="s">
+      <c r="E155" s="117" t="s">
         <v>2321</v>
       </c>
       <c r="F155" s="20" t="s">
@@ -30009,10 +30112,10 @@
       <c r="G155" s="21" t="s">
         <v>2218</v>
       </c>
-      <c r="H155" s="21" t="s">
+      <c r="H155" s="116" t="s">
         <v>149</v>
       </c>
-      <c r="I155" s="118" t="s">
+      <c r="I155" s="116" t="s">
         <v>79</v>
       </c>
     </row>
@@ -30038,7 +30141,7 @@
       <c r="G156" s="21" t="s">
         <v>2223</v>
       </c>
-      <c r="H156" s="118" t="s">
+      <c r="H156" s="127" t="s">
         <v>36</v>
       </c>
       <c r="I156" s="21" t="s">
@@ -30087,10 +30190,10 @@
       <c r="D158" s="50" t="s">
         <v>2332</v>
       </c>
-      <c r="E158" s="18" t="s">
+      <c r="E158" s="117" t="s">
         <v>2333</v>
       </c>
-      <c r="F158" s="20" t="s">
+      <c r="F158" s="144" t="s">
         <v>10</v>
       </c>
       <c r="G158" s="21" t="s">
@@ -30099,7 +30202,7 @@
       <c r="H158" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="I158" s="21" t="s">
+      <c r="I158" s="116" t="s">
         <v>116</v>
       </c>
     </row>
@@ -30116,19 +30219,19 @@
       <c r="D159" s="50" t="s">
         <v>2336</v>
       </c>
-      <c r="E159" s="19" t="s">
+      <c r="E159" s="149" t="s">
         <v>2337</v>
       </c>
-      <c r="F159" s="20" t="s">
+      <c r="F159" s="133" t="s">
         <v>10</v>
       </c>
       <c r="G159" s="21" t="s">
         <v>2274</v>
       </c>
-      <c r="H159" s="118" t="s">
+      <c r="H159" s="116" t="s">
         <v>60</v>
       </c>
-      <c r="I159" s="21" t="s">
+      <c r="I159" s="116" t="s">
         <v>469</v>
       </c>
     </row>
@@ -30152,7 +30255,7 @@
       <c r="G160" s="21" t="s">
         <v>2223</v>
       </c>
-      <c r="H160" s="118" t="s">
+      <c r="H160" s="123" t="s">
         <v>316</v>
       </c>
       <c r="I160" s="21" t="s">
@@ -30184,7 +30287,7 @@
       <c r="H161" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="I161" s="118" t="s">
+      <c r="I161" s="116" t="s">
         <v>253</v>
       </c>
     </row>
@@ -30201,16 +30304,16 @@
       <c r="D162" s="52" t="s">
         <v>2348</v>
       </c>
-      <c r="E162" s="18" t="s">
+      <c r="E162" s="117" t="s">
         <v>2349</v>
       </c>
-      <c r="F162" s="20" t="s">
+      <c r="F162" s="144" t="s">
         <v>10</v>
       </c>
       <c r="G162" s="21" t="s">
         <v>2261</v>
       </c>
-      <c r="H162" s="21" t="s">
+      <c r="H162" s="116" t="s">
         <v>27</v>
       </c>
       <c r="I162" s="21" t="s">
@@ -30259,19 +30362,19 @@
       <c r="D164" s="50" t="s">
         <v>2355</v>
       </c>
-      <c r="E164" s="18" t="s">
+      <c r="E164" s="117" t="s">
         <v>2356</v>
       </c>
-      <c r="F164" s="20" t="s">
+      <c r="F164" s="133" t="s">
         <v>10</v>
       </c>
       <c r="G164" s="21" t="s">
         <v>2218</v>
       </c>
-      <c r="H164" s="21" t="s">
+      <c r="H164" s="116" t="s">
         <v>27</v>
       </c>
-      <c r="I164" s="118" t="s">
+      <c r="I164" s="116" t="s">
         <v>202</v>
       </c>
     </row>
@@ -30297,7 +30400,7 @@
       <c r="G165" s="21" t="s">
         <v>2218</v>
       </c>
-      <c r="H165" s="118" t="s">
+      <c r="H165" s="127" t="s">
         <v>36</v>
       </c>
       <c r="I165" s="21" t="s">
@@ -30326,10 +30429,10 @@
       <c r="G166" s="21" t="s">
         <v>2274</v>
       </c>
-      <c r="H166" s="118" t="s">
+      <c r="H166" s="116" t="s">
         <v>65</v>
       </c>
-      <c r="I166" s="118" t="s">
+      <c r="I166" s="116" t="s">
         <v>202</v>
       </c>
     </row>
@@ -30344,7 +30447,7 @@
       <c r="D167" s="108" t="s">
         <v>2366</v>
       </c>
-      <c r="E167" s="18" t="s">
+      <c r="E167" s="117" t="s">
         <v>2367</v>
       </c>
       <c r="F167" s="20" t="s">
@@ -30353,10 +30456,10 @@
       <c r="G167" s="21" t="s">
         <v>2218</v>
       </c>
-      <c r="H167" s="118" t="s">
+      <c r="H167" s="116" t="s">
         <v>45</v>
       </c>
-      <c r="I167" s="21" t="s">
+      <c r="I167" s="116" t="s">
         <v>561</v>
       </c>
     </row>
@@ -30382,7 +30485,7 @@
       <c r="G168" s="21" t="s">
         <v>2261</v>
       </c>
-      <c r="H168" s="118" t="s">
+      <c r="H168" s="116" t="s">
         <v>65</v>
       </c>
       <c r="I168" s="21" t="s">
@@ -30402,19 +30505,19 @@
       <c r="D169" s="107" t="s">
         <v>2373</v>
       </c>
-      <c r="E169" s="18" t="s">
+      <c r="E169" s="117" t="s">
         <v>2374</v>
       </c>
-      <c r="F169" s="20" t="s">
+      <c r="F169" s="144" t="s">
         <v>10</v>
       </c>
       <c r="G169" s="21" t="s">
         <v>2248</v>
       </c>
-      <c r="H169" s="21" t="s">
+      <c r="H169" s="123" t="s">
         <v>102</v>
       </c>
-      <c r="I169" s="21" t="s">
+      <c r="I169" s="116" t="s">
         <v>116</v>
       </c>
     </row>
@@ -30493,7 +30596,7 @@
       <c r="H172" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="I172" s="118" t="s">
+      <c r="I172" s="116" t="s">
         <v>92</v>
       </c>
     </row>
@@ -30519,10 +30622,10 @@
       <c r="G173" s="21" t="s">
         <v>2261</v>
       </c>
-      <c r="H173" s="118" t="s">
+      <c r="H173" s="127" t="s">
         <v>141</v>
       </c>
-      <c r="I173" s="118" t="s">
+      <c r="I173" s="116" t="s">
         <v>12</v>
       </c>
     </row>
@@ -30551,7 +30654,7 @@
       <c r="H174" s="21" t="s">
         <v>357</v>
       </c>
-      <c r="I174" s="118" t="s">
+      <c r="I174" s="116" t="s">
         <v>92</v>
       </c>
     </row>
@@ -30577,10 +30680,10 @@
       <c r="G175" s="21" t="s">
         <v>2274</v>
       </c>
-      <c r="H175" s="118" t="s">
+      <c r="H175" s="127" t="s">
         <v>141</v>
       </c>
-      <c r="I175" s="118" t="s">
+      <c r="I175" s="123" t="s">
         <v>74</v>
       </c>
     </row>
@@ -30635,7 +30738,7 @@
       <c r="G177" s="21" t="s">
         <v>2223</v>
       </c>
-      <c r="H177" s="118" t="s">
+      <c r="H177" s="116" t="s">
         <v>59</v>
       </c>
       <c r="I177" s="21" t="s">
@@ -30696,7 +30799,7 @@
       <c r="H179" s="21" t="s">
         <v>360</v>
       </c>
-      <c r="I179" s="118" t="s">
+      <c r="I179" s="127" t="s">
         <v>22</v>
       </c>
     </row>
@@ -30751,7 +30854,7 @@
       <c r="G181" s="21" t="s">
         <v>2218</v>
       </c>
-      <c r="H181" s="21" t="s">
+      <c r="H181" s="123" t="s">
         <v>102</v>
       </c>
       <c r="I181" s="21" t="s">
@@ -30780,7 +30883,7 @@
       <c r="G182" s="22" t="s">
         <v>2218</v>
       </c>
-      <c r="H182" s="122" t="s">
+      <c r="H182" s="120" t="s">
         <v>59</v>
       </c>
       <c r="I182" s="22" t="s">
@@ -30841,7 +30944,7 @@
       <c r="H184" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="I184" s="118" t="s">
+      <c r="I184" s="116" t="s">
         <v>253</v>
       </c>
     </row>
@@ -30867,7 +30970,7 @@
       <c r="G185" s="21" t="s">
         <v>2218</v>
       </c>
-      <c r="H185" s="118" t="s">
+      <c r="H185" s="127" t="s">
         <v>22</v>
       </c>
       <c r="I185" s="21" t="s">
@@ -30917,10 +31020,10 @@
       <c r="G187" s="21" t="s">
         <v>2223</v>
       </c>
-      <c r="H187" s="118" t="s">
+      <c r="H187" s="116" t="s">
         <v>45</v>
       </c>
-      <c r="I187" s="118" t="s">
+      <c r="I187" s="123" t="s">
         <v>74</v>
       </c>
     </row>
@@ -30949,7 +31052,7 @@
       <c r="H188" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="I188" s="118" t="s">
+      <c r="I188" s="116" t="s">
         <v>133</v>
       </c>
     </row>
@@ -30966,10 +31069,10 @@
       <c r="D189" s="50" t="s">
         <v>2448</v>
       </c>
-      <c r="E189" s="50" t="s">
+      <c r="E189" s="148" t="s">
         <v>2449</v>
       </c>
-      <c r="F189" s="41" t="s">
+      <c r="F189" s="142" t="s">
         <v>10</v>
       </c>
       <c r="G189" s="21" t="s">
@@ -30978,7 +31081,7 @@
       <c r="H189" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="I189" s="21" t="s">
+      <c r="I189" s="116" t="s">
         <v>111</v>
       </c>
     </row>
@@ -31002,7 +31105,7 @@
         <v>838</v>
       </c>
       <c r="G190" s="23"/>
-      <c r="H190" s="121" t="s">
+      <c r="H190" s="129" t="s">
         <v>36</v>
       </c>
       <c r="I190" s="23" t="s">
@@ -31022,17 +31125,17 @@
       <c r="D191" s="107" t="s">
         <v>2454</v>
       </c>
-      <c r="E191" s="52" t="s">
+      <c r="E191" s="134" t="s">
         <v>2455</v>
       </c>
-      <c r="F191" s="41" t="s">
+      <c r="F191" s="137" t="s">
         <v>838</v>
       </c>
       <c r="G191" s="21"/>
-      <c r="H191" s="121" t="s">
+      <c r="H191" s="119" t="s">
         <v>514</v>
       </c>
-      <c r="I191" s="21" t="s">
+      <c r="I191" s="116" t="s">
         <v>111</v>
       </c>
     </row>
@@ -31056,7 +31159,7 @@
         <v>838</v>
       </c>
       <c r="G192" s="21"/>
-      <c r="H192" s="118" t="s">
+      <c r="H192" s="127" t="s">
         <v>36</v>
       </c>
       <c r="I192" s="21" t="s">
@@ -31083,7 +31186,7 @@
         <v>838</v>
       </c>
       <c r="G193" s="22"/>
-      <c r="H193" s="122" t="s">
+      <c r="H193" s="120" t="s">
         <v>65</v>
       </c>
       <c r="I193" s="21" t="s">
@@ -31110,7 +31213,7 @@
         <v>838</v>
       </c>
       <c r="G194" s="21"/>
-      <c r="H194" s="118" t="s">
+      <c r="H194" s="127" t="s">
         <v>22</v>
       </c>
       <c r="I194" s="21" t="s">
@@ -31139,7 +31242,7 @@
       <c r="G195" s="21" t="s">
         <v>2248</v>
       </c>
-      <c r="H195" s="118" t="s">
+      <c r="H195" s="127" t="s">
         <v>22</v>
       </c>
       <c r="I195" s="21" t="s">
@@ -31197,7 +31300,7 @@
       <c r="G197" s="21" t="s">
         <v>2218</v>
       </c>
-      <c r="H197" s="118" t="s">
+      <c r="H197" s="116" t="s">
         <v>128</v>
       </c>
       <c r="I197" s="21" t="s">
@@ -31226,10 +31329,10 @@
       <c r="G198" s="21" t="s">
         <v>2218</v>
       </c>
-      <c r="H198" s="118" t="s">
+      <c r="H198" s="116" t="s">
         <v>73</v>
       </c>
-      <c r="I198" s="118" t="s">
+      <c r="I198" s="116" t="s">
         <v>193</v>
       </c>
     </row>
@@ -31258,7 +31361,7 @@
       <c r="H199" s="21" t="s">
         <v>270</v>
       </c>
-      <c r="I199" s="122" t="s">
+      <c r="I199" s="120" t="s">
         <v>193</v>
       </c>
     </row>
@@ -31284,10 +31387,10 @@
       <c r="G200" s="21" t="s">
         <v>2291</v>
       </c>
-      <c r="H200" s="118" t="s">
+      <c r="H200" s="116" t="s">
         <v>328</v>
       </c>
-      <c r="I200" s="118" t="s">
+      <c r="I200" s="116" t="s">
         <v>193</v>
       </c>
     </row>
@@ -31304,19 +31407,19 @@
       <c r="D201" s="50" t="s">
         <v>2494</v>
       </c>
-      <c r="E201" s="52" t="s">
+      <c r="E201" s="134" t="s">
         <v>2495</v>
       </c>
-      <c r="F201" s="41" t="s">
+      <c r="F201" s="137" t="s">
         <v>10</v>
       </c>
       <c r="G201" s="21" t="s">
         <v>2223</v>
       </c>
-      <c r="H201" s="118" t="s">
+      <c r="H201" s="123" t="s">
         <v>120</v>
       </c>
-      <c r="I201" s="117" t="s">
+      <c r="I201" s="115" t="s">
         <v>514</v>
       </c>
     </row>
@@ -31333,10 +31436,10 @@
       <c r="D202" s="50" t="s">
         <v>2498</v>
       </c>
-      <c r="E202" s="52" t="s">
+      <c r="E202" s="134" t="s">
         <v>2499</v>
       </c>
-      <c r="F202" s="41" t="s">
+      <c r="F202" s="150" t="s">
         <v>10</v>
       </c>
       <c r="G202" s="21" t="s">
@@ -31345,7 +31448,7 @@
       <c r="H202" s="21" t="s">
         <v>2500</v>
       </c>
-      <c r="I202" s="21" t="s">
+      <c r="I202" s="116" t="s">
         <v>469</v>
       </c>
     </row>
@@ -31449,10 +31552,10 @@
       <c r="D206" s="52" t="s">
         <v>2515</v>
       </c>
-      <c r="E206" s="52" t="s">
+      <c r="E206" s="134" t="s">
         <v>2516</v>
       </c>
-      <c r="F206" s="41" t="s">
+      <c r="F206" s="142" t="s">
         <v>10</v>
       </c>
       <c r="G206" s="21" t="s">
@@ -31461,7 +31564,7 @@
       <c r="H206" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="I206" s="22" t="s">
+      <c r="I206" s="120" t="s">
         <v>111</v>
       </c>
       <c r="J206" s="110"/>
@@ -31678,10 +31781,10 @@
       <c r="G211" s="21" t="s">
         <v>2218</v>
       </c>
-      <c r="H211" s="118" t="s">
+      <c r="H211" s="116" t="s">
         <v>64</v>
       </c>
-      <c r="I211" s="118" t="s">
+      <c r="I211" s="123" t="s">
         <v>120</v>
       </c>
       <c r="J211" s="106"/>
@@ -31725,7 +31828,7 @@
       <c r="H212" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="I212" s="118" t="s">
+      <c r="I212" s="116" t="s">
         <v>79</v>
       </c>
       <c r="J212" s="106"/>
@@ -31769,7 +31872,7 @@
       <c r="H213" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="I213" s="118" t="s">
+      <c r="I213" s="127" t="s">
         <v>22</v>
       </c>
       <c r="J213" s="106"/>
@@ -31845,19 +31948,19 @@
       <c r="D215" s="50" t="s">
         <v>2549</v>
       </c>
-      <c r="E215" s="69" t="s">
+      <c r="E215" s="140" t="s">
         <v>2550</v>
       </c>
-      <c r="F215" s="41" t="s">
+      <c r="F215" s="137" t="s">
         <v>10</v>
       </c>
       <c r="G215" s="21" t="s">
         <v>2248</v>
       </c>
-      <c r="H215" s="118" t="s">
+      <c r="H215" s="116" t="s">
         <v>12</v>
       </c>
-      <c r="I215" s="21" t="s">
+      <c r="I215" s="116" t="s">
         <v>488</v>
       </c>
       <c r="J215" s="106"/>
@@ -31889,10 +31992,10 @@
       <c r="D216" s="50" t="s">
         <v>2553</v>
       </c>
-      <c r="E216" s="54" t="s">
+      <c r="E216" s="141" t="s">
         <v>2554</v>
       </c>
-      <c r="F216" s="41" t="s">
+      <c r="F216" s="137" t="s">
         <v>10</v>
       </c>
       <c r="G216" s="21" t="s">
@@ -31901,7 +32004,7 @@
       <c r="H216" s="21" t="s">
         <v>2345</v>
       </c>
-      <c r="I216" s="21" t="s">
+      <c r="I216" s="116" t="s">
         <v>488</v>
       </c>
       <c r="J216" s="106"/>
@@ -31945,7 +32048,7 @@
       <c r="H217" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="I217" s="118" t="s">
+      <c r="I217" s="116" t="s">
         <v>431</v>
       </c>
       <c r="J217" s="106"/>
@@ -32021,10 +32124,10 @@
       <c r="D219" s="108" t="s">
         <v>2564</v>
       </c>
-      <c r="E219" s="52" t="s">
+      <c r="E219" s="134" t="s">
         <v>2565</v>
       </c>
-      <c r="F219" s="41" t="s">
+      <c r="F219" s="142" t="s">
         <v>10</v>
       </c>
       <c r="G219" s="40" t="s">
@@ -32033,7 +32136,7 @@
       <c r="H219" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="I219" s="21" t="s">
+      <c r="I219" s="116" t="s">
         <v>488</v>
       </c>
       <c r="J219" s="106"/>
@@ -32074,7 +32177,7 @@
       <c r="G220" s="21" t="s">
         <v>2274</v>
       </c>
-      <c r="H220" s="118" t="s">
+      <c r="H220" s="127" t="s">
         <v>36</v>
       </c>
       <c r="I220" s="21" t="s">
@@ -32109,7 +32212,7 @@
       <c r="D221" s="50" t="s">
         <v>2572</v>
       </c>
-      <c r="E221" s="52" t="s">
+      <c r="E221" s="134" t="s">
         <v>2573</v>
       </c>
       <c r="F221" s="41" t="s">
@@ -32118,7 +32221,7 @@
       <c r="G221" s="21" t="s">
         <v>2248</v>
       </c>
-      <c r="H221" s="21" t="s">
+      <c r="H221" s="116" t="s">
         <v>106</v>
       </c>
       <c r="I221" s="21" t="s">
@@ -32153,7 +32256,7 @@
       <c r="D222" s="50" t="s">
         <v>2576</v>
       </c>
-      <c r="E222" s="52" t="s">
+      <c r="E222" s="134" t="s">
         <v>2577</v>
       </c>
       <c r="F222" s="41" t="s">
@@ -32162,10 +32265,10 @@
       <c r="G222" s="21" t="s">
         <v>2248</v>
       </c>
-      <c r="H222" s="118" t="s">
+      <c r="H222" s="116" t="s">
         <v>128</v>
       </c>
-      <c r="I222" s="21" t="s">
+      <c r="I222" s="116" t="s">
         <v>111</v>
       </c>
       <c r="J222" s="106"/>
@@ -32197,10 +32300,10 @@
       <c r="D223" s="50" t="s">
         <v>2580</v>
       </c>
-      <c r="E223" s="52" t="s">
+      <c r="E223" s="134" t="s">
         <v>2581</v>
       </c>
-      <c r="F223" s="41" t="s">
+      <c r="F223" s="142" t="s">
         <v>10</v>
       </c>
       <c r="G223" s="21" t="s">
@@ -32209,7 +32312,7 @@
       <c r="H223" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="I223" s="21" t="s">
+      <c r="I223" s="116" t="s">
         <v>41</v>
       </c>
       <c r="J223" s="106"/>
@@ -32253,7 +32356,7 @@
       <c r="H224" s="40" t="s">
         <v>844</v>
       </c>
-      <c r="I224" s="120" t="s">
+      <c r="I224" s="130" t="s">
         <v>36</v>
       </c>
       <c r="J224" s="1"/>
@@ -32285,7 +32388,7 @@
       <c r="D225" s="112" t="s">
         <v>2587</v>
       </c>
-      <c r="E225" s="113" t="s">
+      <c r="E225" s="135" t="s">
         <v>2588</v>
       </c>
       <c r="F225" s="71" t="s">
@@ -32294,10 +32397,10 @@
       <c r="G225" s="40" t="s">
         <v>2218</v>
       </c>
-      <c r="H225" s="40" t="s">
+      <c r="H225" s="118" t="s">
         <v>106</v>
       </c>
-      <c r="I225" s="120" t="s">
+      <c r="I225" s="118" t="s">
         <v>253</v>
       </c>
       <c r="J225" s="1"/>
@@ -32374,7 +32477,7 @@
       <c r="H227" s="40" t="s">
         <v>1738</v>
       </c>
-      <c r="I227" s="120" t="s">
+      <c r="I227" s="118" t="s">
         <v>253</v>
       </c>
       <c r="J227" s="106"/>

</xml_diff>